<commit_message>
feature and reward statistics added + plots
</commit_message>
<xml_diff>
--- a/configs_rl.xlsx
+++ b/configs_rl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reizinger Patrik\Documents\GitHub\GANerated-curiosity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD38D5F-07FB-4152-B388-617817ED49B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39DC3E2-AE7C-4051-AD10-0B4C3C394CCC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{197C701C-957C-4E8C-9796-037C7C4CDE85}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="24">
   <si>
     <t>env</t>
   </si>
@@ -499,7 +499,7 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,10 +629,10 @@
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -653,10 +653,10 @@
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -773,7 +773,9 @@
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -795,7 +797,9 @@
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -842,7 +846,9 @@
         <v>9</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -864,7 +870,9 @@
         <v>9</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -886,7 +894,9 @@
         <v>9</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -908,7 +918,9 @@
         <v>9</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -930,7 +942,9 @@
         <v>9</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -952,7 +966,9 @@
         <v>9</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>